<commit_message>
access level and basic  admin a/c created '
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/02-BulkUploadEmployee.xlsx
+++ b/documents/templates/bulk-upload/02-BulkUploadEmployee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF99E2D-C2B2-E941-903F-9312B21BE13B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CF511E-51FD-3244-B0DE-C55E63F0E2C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{6BA803BE-7637-644E-81BF-475A654E4F59}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Notify for Machine Maintenance</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Employee Id</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -403,15 +412,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC00F89-2235-B741-A22E-475A64033711}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -437,6 +450,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>